<commit_message>
Made corrections after the review
</commit_message>
<xml_diff>
--- a/wines.xlsx
+++ b/wines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kit/Development/DEVMAN/wine-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6D6B5D-444E-6D4A-A67C-E9B16695A5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB369C1F-E22E-7E40-943A-5E7CCDE8BCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Название</t>
   </si>
@@ -43,12 +43,6 @@
     <t>belaya_ledi.png</t>
   </si>
   <si>
-    <t>Ркацители</t>
-  </si>
-  <si>
-    <t>rkaciteli.png</t>
-  </si>
-  <si>
     <t>Хванчкара</t>
   </si>
   <si>
@@ -91,25 +85,10 @@
     <t>kokur.png</t>
   </si>
   <si>
-    <t>Киндзмараули</t>
-  </si>
-  <si>
-    <t>Саперави</t>
-  </si>
-  <si>
-    <t>kindzmarauli.png</t>
-  </si>
-  <si>
     <t>Чача</t>
   </si>
   <si>
     <t>chacha.png</t>
-  </si>
-  <si>
-    <t>Коньяк кизиловый</t>
-  </si>
-  <si>
-    <t>konyak_kizilovyi.png</t>
   </si>
   <si>
     <t>Акция</t>
@@ -403,10 +382,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -420,7 +399,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -435,12 +414,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -455,148 +434,104 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
         <v>350</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4">
-        <v>499</v>
+        <v>399</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4">
-        <v>399</v>
+        <v>550</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4">
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="4">
-        <v>450</v>
+        <v>299</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="4">
-        <v>550</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
-        <v>299</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
-        <v>350</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>